<commit_message>
Added Automatic Data Visualization
</commit_message>
<xml_diff>
--- a/SRC/Dps.xlsx
+++ b/SRC/Dps.xlsx
@@ -13458,12 +13458,24 @@
           <t>99.9</t>
         </is>
       </c>
+      <c r="B1001" t="n">
+        <v>817385</v>
+      </c>
+      <c r="C1001" t="n">
+        <v>1859338</v>
+      </c>
     </row>
     <row r="1002" ht="18.75" customHeight="1">
       <c r="A1002" s="3" t="inlineStr">
         <is>
           <t>100.0</t>
         </is>
+      </c>
+      <c r="B1002" t="n">
+        <v>817385</v>
+      </c>
+      <c r="C1002" t="n">
+        <v>1859338</v>
       </c>
     </row>
     <row r="1003" ht="18.75" customHeight="1">

</xml_diff>